<commit_message>
Finished scraping colleges, need to add majors still
</commit_message>
<xml_diff>
--- a/requirements/grading_sheet.xlsx
+++ b/requirements/grading_sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omar/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omar/Desktop/CSE416/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6058B41E-0132-784C-AB72-E275AC2781F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B446296-575A-344A-AC16-1B5882AF6344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8880" yWindow="3000" windowWidth="21600" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>POINTS</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>6.3 Search for colleges.  filters 10pts; sorting 3pts; modify search 2pts; the rest 4pts.</t>
+  </si>
+  <si>
+    <t>j</t>
   </si>
 </sst>
 </file>
@@ -341,7 +344,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -364,6 +366,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -765,17 +770,19 @@
       <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="21">
         <v>3</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="8">
+        <v>3</v>
+      </c>
       <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="8">
@@ -785,7 +792,7 @@
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="8">
@@ -795,7 +802,7 @@
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="8">
@@ -805,10 +812,10 @@
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="21">
         <v>11</v>
       </c>
       <c r="C10" s="8"/>
@@ -857,72 +864,84 @@
       <c r="D15" s="8"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="21">
         <v>3</v>
       </c>
-      <c r="C16" s="22"/>
+      <c r="C16" s="21">
+        <v>3</v>
+      </c>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="25" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B17" s="25">
         <v>3</v>
       </c>
-      <c r="C17" s="26"/>
+      <c r="C17" s="25">
+        <v>3</v>
+      </c>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A18" s="23" t="s">
+    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A18" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="21">
         <v>5</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="21">
+        <v>5</v>
+      </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="25" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B19" s="21">
         <v>2</v>
       </c>
-      <c r="C19" s="26"/>
+      <c r="C19" s="21">
+        <v>2</v>
+      </c>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="25" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="21">
         <v>3</v>
       </c>
-      <c r="C20" s="26"/>
+      <c r="C20" s="21">
+        <v>3</v>
+      </c>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="14" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="21">
         <v>3</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="21">
+        <v>3</v>
+      </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="9"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="10" t="s">
         <v>15</v>
       </c>
@@ -930,17 +949,17 @@
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="27" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B24" s="27">
         <v>4</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-    </row>
-    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+    </row>
+    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
         <v>14</v>
       </c>
@@ -950,7 +969,7 @@
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
         <v>16</v>
       </c>
@@ -960,51 +979,54 @@
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="20" t="s">
+    <row r="27" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="14">
         <v>2</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="14">
         <v>2</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="15"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" s="10"/>
-      <c r="B30" s="15"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="10"/>
-      <c r="B32" s="15"/>
+      <c r="B32" s="14"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
@@ -1032,12 +1054,12 @@
       <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="2"/>

</xml_diff>

<commit_message>
Generate students + hw6
</commit_message>
<xml_diff>
--- a/requirements/grading_sheet.xlsx
+++ b/requirements/grading_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omar/Desktop/CSE416/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B446296-575A-344A-AC16-1B5882AF6344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED8C79A-5B19-4344-9AC5-B38043C77606}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8880" yWindow="3000" windowWidth="21600" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3780" yWindow="2540" windowWidth="27380" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,45 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={7AEF54F4-86B4-D646-B500-6CC701DE51A3}</author>
+    <author>tc={8229F1FB-6008-7A4D-BEDE-4E92A69F689B}</author>
+    <author>tc={E5BCCA63-2A32-6F4E-ACB7-E1C617DB9AC9}</author>
+  </authors>
+  <commentList>
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{7AEF54F4-86B4-D646-B500-6CC701DE51A3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Sorting is implemented, 
+Filters do not support locations and majors yet</t>
+      </text>
+    </comment>
+    <comment ref="C24" authorId="1" shapeId="0" xr:uid="{8229F1FB-6008-7A4D-BEDE-4E92A69F689B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Passwords are salted and hashed, but authorization still needs implementation</t>
+      </text>
+    </comment>
+    <comment ref="C25" authorId="2" shapeId="0" xr:uid="{E5BCCA63-2A32-6F4E-ACB7-E1C617DB9AC9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Django already takes care of this</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>POINTS</t>
   </si>
@@ -37,9 +74,6 @@
   </si>
   <si>
     <t>POSSIBLE</t>
-  </si>
-  <si>
-    <t>Main languages and technologies:</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -146,14 +180,14 @@
     <t>6.3 Search for colleges.  filters 10pts; sorting 3pts; modify search 2pts; the rest 4pts.</t>
   </si>
   <si>
-    <t>j</t>
+    <t>Main languages and technologies: Python, React</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -179,8 +213,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,13 +235,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -361,14 +395,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,6 +415,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Omar Amin" id="{03CC5D12-F035-E04C-AD7F-F8E518026EB4}" userId="S::omar.amin@stonybrook.edu::1cff5511-39db-417e-89c4-7d8f0786568c" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -705,31 +742,46 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C8" dT="2020-03-26T17:45:58.07" personId="{03CC5D12-F035-E04C-AD7F-F8E518026EB4}" id="{7AEF54F4-86B4-D646-B500-6CC701DE51A3}">
+    <text>Sorting is implemented, 
+Filters do not support locations and majors yet</text>
+  </threadedComment>
+  <threadedComment ref="C24" dT="2020-03-26T17:47:28.81" personId="{03CC5D12-F035-E04C-AD7F-F8E518026EB4}" id="{8229F1FB-6008-7A4D-BEDE-4E92A69F689B}">
+    <text>Passwords are salted and hashed, but authorization still needs implementation</text>
+  </threadedComment>
+  <threadedComment ref="C25" dT="2020-03-26T17:46:49.04" personId="{03CC5D12-F035-E04C-AD7F-F8E518026EB4}" id="{E5BCCA63-2A32-6F4E-ACB7-E1C617DB9AC9}">
+    <text>Django already takes care of this</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="74.33203125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -749,7 +801,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -763,27 +815,27 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A6" s="28" t="s">
-        <v>9</v>
+      <c r="A6" s="23" t="s">
+        <v>8</v>
       </c>
       <c r="B6" s="21">
         <v>3</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="21">
         <v>3</v>
       </c>
       <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="8">
         <v>9</v>
@@ -792,18 +844,20 @@
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="8">
+      <c r="A8" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="21">
         <v>19</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="21">
+        <v>8</v>
+      </c>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="8">
         <v>7</v>
@@ -812,18 +866,18 @@
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="21">
+      <c r="A10" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="24">
         <v>11</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="8">
         <v>6</v>
@@ -833,7 +887,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="8">
         <v>11</v>
@@ -843,7 +897,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -857,7 +911,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -865,7 +919,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="21">
         <v>3</v>
@@ -875,21 +929,21 @@
       </c>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="21">
         <v>3</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="21">
         <v>3</v>
       </c>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="21">
         <v>5</v>
@@ -899,9 +953,9 @@
       </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="21">
         <v>2</v>
@@ -911,9 +965,9 @@
       </c>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="21">
         <v>3</v>
@@ -923,9 +977,9 @@
       </c>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="21">
         <v>3</v>
@@ -935,43 +989,47 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="9"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="26" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="21">
+        <v>4</v>
+      </c>
+      <c r="C24" s="21">
+        <v>2</v>
+      </c>
+      <c r="D24" s="24"/>
+    </row>
+    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="27">
-        <v>4</v>
-      </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-    </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="9">
+      <c r="B25" s="20">
         <v>2</v>
       </c>
-      <c r="C25" s="10"/>
+      <c r="C25" s="20">
+        <v>2</v>
+      </c>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="8">
         <v>5</v>
@@ -979,22 +1037,19 @@
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" s="14">
         <v>2</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-      <c r="G27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="14">
         <v>2</v>
@@ -1002,29 +1057,29 @@
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="10"/>
       <c r="B30" s="14"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31" s="14"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="10"/>
       <c r="B32" s="14"/>
       <c r="C32" s="8"/>
@@ -1044,18 +1099,20 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35" s="8">
         <f>SUM(B1:B34)</f>
         <v>100</v>
       </c>
-      <c r="C35" s="8"/>
+      <c r="C35" s="8">
+        <v>34</v>
+      </c>
       <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="17" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -1074,5 +1131,6 @@
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>